<commit_message>
hunting user profile 70% completed
</commit_message>
<xml_diff>
--- a/usernames_dummy.xlsx
+++ b/usernames_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujal Karmakar\Desktop\Desktop\Data Analyst\Instagram Data Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6492AD-DAC5-45E8-BB7B-87630C9847A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E214679A-137F-48F2-B43F-655F3F5EFB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="1248" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>sujal.incognito</t>
+  </si>
+  <si>
+    <t>leomessi</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,6 +425,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
all bio details function completed
</commit_message>
<xml_diff>
--- a/usernames_dummy.xlsx
+++ b/usernames_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujal Karmakar\Desktop\Desktop\Data Analyst\Instagram Data Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E214679A-137F-48F2-B43F-655F3F5EFB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11EC0D-BAC3-4531-8710-69D7088B593C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="1248" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>dylankato</t>
   </si>
   <si>
     <t>just.sujal.yk</t>
@@ -397,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,17 +414,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed auto injection of external links by IG
</commit_message>
<xml_diff>
--- a/usernames_dummy.xlsx
+++ b/usernames_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujal Karmakar\Desktop\Desktop\Data Analyst\Instagram Data Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11EC0D-BAC3-4531-8710-69D7088B593C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0545727-FD85-4356-9043-009B16770520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="1248" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>leomessi</t>
+  </si>
+  <si>
+    <t>__sanatani__090</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,6 +425,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed few single link which was not being targeted due to the presence of thread link
</commit_message>
<xml_diff>
--- a/usernames_dummy.xlsx
+++ b/usernames_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujal Karmakar\Desktop\Desktop\Data Analyst\Instagram Data Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0545727-FD85-4356-9043-009B16770520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FA0550-15E2-41A5-B530-CEF10B929734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="1248" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,16 @@
     <t>Username</t>
   </si>
   <si>
-    <t>just.sujal.yk</t>
+    <t>__sanatani__090</t>
   </si>
   <si>
-    <t>sujal.incognito</t>
+    <t>_abo_safwan_</t>
   </si>
   <si>
-    <t>leomessi</t>
+    <t>__r_n_shanawar__</t>
   </si>
   <si>
-    <t>__sanatani__090</t>
+    <t>_agencia.dara</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,12 +417,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
saving to excel done
</commit_message>
<xml_diff>
--- a/usernames_dummy.xlsx
+++ b/usernames_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujal Karmakar\Desktop\Desktop\Data Analyst\Instagram Data Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B236C0-9DEF-4C00-9535-BCF96AB4B4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE051194-D577-4AE9-8A03-CFCDCDBE4A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
   <si>
     <t>Username</t>
   </si>
@@ -44,6 +44,342 @@
   </si>
   <si>
     <t>_agencia.dara</t>
+  </si>
+  <si>
+    <t>simplyshabd</t>
+  </si>
+  <si>
+    <t>apoorvajadaun</t>
+  </si>
+  <si>
+    <t>rashi_lunia</t>
+  </si>
+  <si>
+    <t>explorerbhavana</t>
+  </si>
+  <si>
+    <t>anuj_._.__</t>
+  </si>
+  <si>
+    <t>tci_theclassyissue</t>
+  </si>
+  <si>
+    <t>aava_rai</t>
+  </si>
+  <si>
+    <t>bydastann</t>
+  </si>
+  <si>
+    <t>jushtikaji</t>
+  </si>
+  <si>
+    <t>teekhabanao</t>
+  </si>
+  <si>
+    <t>suzana_pakhrin</t>
+  </si>
+  <si>
+    <t>_samu__22_</t>
+  </si>
+  <si>
+    <t>raj__dhebariya</t>
+  </si>
+  <si>
+    <t>its.raadhaa</t>
+  </si>
+  <si>
+    <t>rohshah</t>
+  </si>
+  <si>
+    <t>kevvu_keka_memes</t>
+  </si>
+  <si>
+    <t>nainaswami_</t>
+  </si>
+  <si>
+    <t>dikulwedding</t>
+  </si>
+  <si>
+    <t>the_taklaboy</t>
+  </si>
+  <si>
+    <t>ashi_z11</t>
+  </si>
+  <si>
+    <t>priyanshu_extraa</t>
+  </si>
+  <si>
+    <t>mr_laniang</t>
+  </si>
+  <si>
+    <t>karimov_5nd</t>
+  </si>
+  <si>
+    <t>nicolettecallie</t>
+  </si>
+  <si>
+    <t>yuripomo</t>
+  </si>
+  <si>
+    <t>dr.yokesharul</t>
+  </si>
+  <si>
+    <t>p3prajyot</t>
+  </si>
+  <si>
+    <t>harrisonniap</t>
+  </si>
+  <si>
+    <t>jay.bevs</t>
+  </si>
+  <si>
+    <t>ranveerallahbadia</t>
+  </si>
+  <si>
+    <t>__rimjhimmm_s</t>
+  </si>
+  <si>
+    <t>dunklift1</t>
+  </si>
+  <si>
+    <t>aditya.thakare21</t>
+  </si>
+  <si>
+    <t>himu_filmz</t>
+  </si>
+  <si>
+    <t>thegridin</t>
+  </si>
+  <si>
+    <t>rashu_dobriyal</t>
+  </si>
+  <si>
+    <t>relatableframe</t>
+  </si>
+  <si>
+    <t>anandharsh610</t>
+  </si>
+  <si>
+    <t>priyanshu_verse</t>
+  </si>
+  <si>
+    <t>adarshuc</t>
+  </si>
+  <si>
+    <t>ashh_lifts_</t>
+  </si>
+  <si>
+    <t>the_booksmiths</t>
+  </si>
+  <si>
+    <t>lolians7</t>
+  </si>
+  <si>
+    <t>vickypatil__</t>
+  </si>
+  <si>
+    <t>oleki_vfx</t>
+  </si>
+  <si>
+    <t>krithisworld</t>
+  </si>
+  <si>
+    <t>trade.core</t>
+  </si>
+  <si>
+    <t>0_anubhya_0</t>
+  </si>
+  <si>
+    <t>carewellington</t>
+  </si>
+  <si>
+    <t>rahulkainthh</t>
+  </si>
+  <si>
+    <t>anee__shaa__</t>
+  </si>
+  <si>
+    <t>manishkharage</t>
+  </si>
+  <si>
+    <t>janhv.i_05</t>
+  </si>
+  <si>
+    <t>shlok__52</t>
+  </si>
+  <si>
+    <t>failicyy</t>
+  </si>
+  <si>
+    <t>aorus_eu</t>
+  </si>
+  <si>
+    <t>iamyoungsaturn</t>
+  </si>
+  <si>
+    <t>prakritisingh____</t>
+  </si>
+  <si>
+    <t>__riseofsigma__</t>
+  </si>
+  <si>
+    <t>aashna_sharma</t>
+  </si>
+  <si>
+    <t>deep.jethwa.397</t>
+  </si>
+  <si>
+    <t>rajsi.underscore</t>
+  </si>
+  <si>
+    <t>officialrajatchauhan</t>
+  </si>
+  <si>
+    <t>_tanishqasahni_</t>
+  </si>
+  <si>
+    <t>ruhisfoodmagic</t>
+  </si>
+  <si>
+    <t>wise_guy_mentality</t>
+  </si>
+  <si>
+    <t>hanzolifts_</t>
+  </si>
+  <si>
+    <t>farzi_aesthetic</t>
+  </si>
+  <si>
+    <t>siddhant.indiavlogs</t>
+  </si>
+  <si>
+    <t>himanikahumour</t>
+  </si>
+  <si>
+    <t>sorted_guy</t>
+  </si>
+  <si>
+    <t>shishirrjhaa</t>
+  </si>
+  <si>
+    <t>isaacbradshaw45</t>
+  </si>
+  <si>
+    <t>dr.rakshita_singh</t>
+  </si>
+  <si>
+    <t>sweat_arena_zone</t>
+  </si>
+  <si>
+    <t>pratikshakhedkar25</t>
+  </si>
+  <si>
+    <t>ronit16_01</t>
+  </si>
+  <si>
+    <t>the.socialpoppers</t>
+  </si>
+  <si>
+    <t>goatedmemes.in</t>
+  </si>
+  <si>
+    <t>lord_amara</t>
+  </si>
+  <si>
+    <t>beyond_with_archan</t>
+  </si>
+  <si>
+    <t>aqsamanzoor._</t>
+  </si>
+  <si>
+    <t>rochit__singh</t>
+  </si>
+  <si>
+    <t>heartify.brainn</t>
+  </si>
+  <si>
+    <t>guriibolte</t>
+  </si>
+  <si>
+    <t>opapacapim_dinho</t>
+  </si>
+  <si>
+    <t>hello.ym_ty</t>
+  </si>
+  <si>
+    <t>estoyiyra</t>
+  </si>
+  <si>
+    <t>jungsanx</t>
+  </si>
+  <si>
+    <t>jenuine_penguin</t>
+  </si>
+  <si>
+    <t>marziis_</t>
+  </si>
+  <si>
+    <t>yourjolpora</t>
+  </si>
+  <si>
+    <t>iiiimohit</t>
+  </si>
+  <si>
+    <t>alinjohhn</t>
+  </si>
+  <si>
+    <t>jack.scalise</t>
+  </si>
+  <si>
+    <t>arhamchordiaa</t>
+  </si>
+  <si>
+    <t>jaichandrap_</t>
+  </si>
+  <si>
+    <t>speedykingh</t>
+  </si>
+  <si>
+    <t>arpitkhajuria_</t>
+  </si>
+  <si>
+    <t>thefilmybomb</t>
+  </si>
+  <si>
+    <t>ash_mogs_</t>
+  </si>
+  <si>
+    <t>sa9irul</t>
+  </si>
+  <si>
+    <t>shams_faraz</t>
+  </si>
+  <si>
+    <t>obxto.amv_18</t>
+  </si>
+  <si>
+    <t>kartikkwadhwa</t>
+  </si>
+  <si>
+    <t>eat_jinjin_dc</t>
+  </si>
+  <si>
+    <t>thriveinit</t>
+  </si>
+  <si>
+    <t>ocastrin</t>
+  </si>
+  <si>
+    <t>riobajracharya</t>
+  </si>
+  <si>
+    <t>baatcheetwithyuvaa</t>
+  </si>
+  <si>
+    <t>ritikumarr_</t>
+  </si>
+  <si>
+    <t>gktrickindia</t>
   </si>
 </sst>
 </file>
@@ -406,15 +742,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="O122" sqref="O122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -460,6 +796,698 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
hunt profile data all done
</commit_message>
<xml_diff>
--- a/usernames_dummy.xlsx
+++ b/usernames_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujal Karmakar\Desktop\Desktop\Data Analyst\Instagram Data Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE051194-D577-4AE9-8A03-CFCDCDBE4A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FA1093-A9C4-49EC-ACDD-E5F7149FD555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
   <si>
     <t>Username</t>
   </si>
@@ -423,9 +423,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -444,7 +442,50 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -455,6 +496,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03C375BF-7364-486B-9FB1-F7D467A809B5}" name="Table1" displayName="Table1" ref="A1:C133" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:C133" xr:uid="{03C375BF-7364-486B-9FB1-F7D467A809B5}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F29495AC-31DD-4431-9D22-ECFB0D186E4E}" name="Username"/>
+    <tableColumn id="2" xr3:uid="{30A2D205-B8A5-4B58-9AE8-D5A0D29E40E1}" name="is_profile_data_fetched"/>
+    <tableColumn id="3" xr3:uid="{76127DE4-E709-4919-B80C-DD9A2B660F86}" name="is_content_data_fetched"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -742,15 +795,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="O122" sqref="O122"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="M122" sqref="M122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -952,543 +1007,878 @@
       <c r="A25" t="s">
         <v>27</v>
       </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>119</v>
       </c>
+      <c r="B132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>81</v>
+      </c>
+      <c r="B133" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>